<commit_message>
Added French concessive data and code to check condition counts
</commit_message>
<xml_diff>
--- a/survey/xiang_kuperberg_ita_2.xlsx
+++ b/survey/xiang_kuperberg_ita_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herts\OneDrive\Desktop\Manu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herts\OneDrive\Desktop\Manu\connectives\survey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9246D8-F583-48B4-97DC-18EFF0F4BC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7002C6F7-AE26-42B9-AFDC-9D15D009DFD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="630" windowWidth="19190" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="0" windowWidth="19160" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2523,7 +2523,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2801,13 +2812,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F629"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A616" workbookViewId="0">
+      <selection activeCell="C232" sqref="C232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="16.26953125" customWidth="1"/>
+    <col min="3" max="3" width="126.54296875" customWidth="1"/>
     <col min="4" max="4" width="18.1796875" customWidth="1"/>
     <col min="5" max="5" width="14.26953125" customWidth="1"/>
     <col min="6" max="6" width="12.08984375" customWidth="1"/>
@@ -13534,6 +13545,9 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>